<commit_message>
Update header styling, date formatting, and filter out template sheets
</commit_message>
<xml_diff>
--- a/LOGC_Tracker.xlsx
+++ b/LOGC_Tracker.xlsx
@@ -8,25 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a9153f6611ebe33/Documents/Hunting Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="520" documentId="8_{29F3ABBB-D82D-4D93-83B8-9233ECB04D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF4739E8-C42F-49D2-B66E-29EB44ADCFAD}"/>
+  <xr:revisionPtr revIDLastSave="583" documentId="8_{29F3ABBB-D82D-4D93-83B8-9233ECB04D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C27C0E88-2314-4329-B9C2-696C8028480F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{FDA17AAC-9089-415D-B005-ED1660AC87E8}"/>
   </bookViews>
   <sheets>
-    <sheet name="11_15_25" sheetId="15" r:id="rId1"/>
-    <sheet name="11_12_25" sheetId="14" r:id="rId2"/>
-    <sheet name="11_9_25" sheetId="13" r:id="rId3"/>
-    <sheet name="11_8_25" sheetId="12" r:id="rId4"/>
-    <sheet name="11_5_25" sheetId="11" r:id="rId5"/>
-    <sheet name="11_2_25" sheetId="10" r:id="rId6"/>
-    <sheet name="11_1_25" sheetId="9" r:id="rId7"/>
-    <sheet name="10_29_25" sheetId="8" r:id="rId8"/>
-    <sheet name="10_26_25" sheetId="7" r:id="rId9"/>
-    <sheet name="10_25_25" sheetId="6" r:id="rId10"/>
-    <sheet name="10_22_25" sheetId="5" r:id="rId11"/>
-    <sheet name="10_19_25" sheetId="4" r:id="rId12"/>
-    <sheet name="10_18_25" sheetId="2" r:id="rId13"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId14"/>
+    <sheet name="11_22_25 TODO" sheetId="18" r:id="rId1"/>
+    <sheet name="11_19_25" sheetId="17" r:id="rId2"/>
+    <sheet name="11_16_25" sheetId="16" r:id="rId3"/>
+    <sheet name="11_15_25" sheetId="15" r:id="rId4"/>
+    <sheet name="11_12_25" sheetId="14" r:id="rId5"/>
+    <sheet name="11_9_25" sheetId="13" r:id="rId6"/>
+    <sheet name="11_8_25" sheetId="12" r:id="rId7"/>
+    <sheet name="11_5_25" sheetId="11" r:id="rId8"/>
+    <sheet name="11_2_25" sheetId="10" r:id="rId9"/>
+    <sheet name="11_1_25" sheetId="9" r:id="rId10"/>
+    <sheet name="10_29_25" sheetId="8" r:id="rId11"/>
+    <sheet name="10_26_25" sheetId="7" r:id="rId12"/>
+    <sheet name="10_25_25" sheetId="6" r:id="rId13"/>
+    <sheet name="10_22_25" sheetId="5" r:id="rId14"/>
+    <sheet name="10_19_25" sheetId="4" r:id="rId15"/>
+    <sheet name="10_18_25" sheetId="2" r:id="rId16"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="62">
   <si>
     <t>Member</t>
   </si>
@@ -226,6 +229,15 @@
   </si>
   <si>
     <t>N 5-7 mph</t>
+  </si>
+  <si>
+    <t>SSE 12-15 mph</t>
+  </si>
+  <si>
+    <t>Cloudy light rain</t>
+  </si>
+  <si>
+    <t>Gray dome</t>
   </si>
 </sst>
 </file>
@@ -774,11 +786,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCD1FAE-E10A-49B0-9459-DEB3D3947B05}">
-  <dimension ref="B2:R17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7548CB-591B-437C-829E-1AFE6F4F8FA2}">
+  <dimension ref="B2:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,14 +856,17 @@
         <v>41</v>
       </c>
       <c r="R2" s="18">
-        <v>45976</v>
+        <v>45983</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1"/>
+      <c r="D3" s="9">
+        <v>7</v>
+      </c>
       <c r="E3" s="7"/>
       <c r="O3" s="13">
         <f>SUM(F3:N3)</f>
@@ -860,15 +875,16 @@
       <c r="Q3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="17">
-        <v>63</v>
-      </c>
+      <c r="R3" s="17"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1"/>
+      <c r="D4" s="9">
+        <v>42</v>
+      </c>
       <c r="E4" s="7"/>
       <c r="O4" s="13">
         <f t="shared" ref="O4:O16" si="0">SUM(F4:N4)</f>
@@ -877,135 +893,82 @@
       <c r="Q4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="17">
-        <v>46</v>
-      </c>
+      <c r="R4" s="17"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="9">
-        <v>7</v>
-      </c>
-      <c r="E5" s="7">
-        <v>2</v>
-      </c>
-      <c r="F5" s="9">
-        <v>14</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E5" s="7"/>
       <c r="O5" s="13">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="R5" s="17" t="s">
-        <v>58</v>
-      </c>
+      <c r="R5" s="17"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="9">
-        <v>41</v>
-      </c>
-      <c r="E6" s="7">
-        <v>4</v>
-      </c>
-      <c r="F6" s="9">
-        <v>3</v>
-      </c>
-      <c r="G6" s="9">
-        <v>1</v>
-      </c>
-      <c r="H6" s="9">
-        <v>1</v>
-      </c>
-      <c r="L6" s="9">
-        <v>3</v>
-      </c>
-      <c r="M6" s="9">
-        <v>2</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E6" s="7"/>
       <c r="O6" s="13">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="R6" s="17" t="s">
-        <v>36</v>
-      </c>
+      <c r="R6" s="17"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="9">
-        <v>18</v>
-      </c>
-      <c r="E7" s="7">
-        <v>3</v>
-      </c>
-      <c r="F7" s="9">
-        <v>2</v>
-      </c>
-      <c r="J7" s="9">
-        <v>1</v>
-      </c>
-      <c r="K7" s="9">
-        <v>2</v>
-      </c>
-      <c r="L7" s="9">
-        <v>9</v>
-      </c>
+      <c r="E7" s="7"/>
       <c r="O7" s="13">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="R7" s="9"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="9">
-        <v>42</v>
-      </c>
-      <c r="E8" s="7">
-        <v>2</v>
-      </c>
-      <c r="F8" s="9">
-        <v>5</v>
-      </c>
-      <c r="L8" s="9">
-        <v>2</v>
-      </c>
+      <c r="E8" s="7"/>
       <c r="O8" s="13">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="4" t="s">
         <v>40</v>
       </c>
       <c r="R8" s="10">
         <f>SUM(F17:L17)</f>
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1"/>
+      <c r="D9" s="9">
+        <v>46</v>
+      </c>
       <c r="E9" s="7"/>
       <c r="O9" s="13">
         <f t="shared" si="0"/>
@@ -1016,14 +979,17 @@
       </c>
       <c r="R9" s="10">
         <f>SUM(F17:G17)</f>
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1"/>
+      <c r="D10" s="9">
+        <v>41</v>
+      </c>
       <c r="E10" s="7"/>
       <c r="O10" s="13">
         <f t="shared" si="0"/>
@@ -1034,12 +1000,12 @@
       </c>
       <c r="R10" s="10">
         <f>SUM(M17)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1"/>
       <c r="E11" s="7"/>
@@ -1050,7 +1016,7 @@
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1"/>
       <c r="E12" s="7"/>
@@ -1061,7 +1027,7 @@
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1"/>
       <c r="E13" s="7"/>
@@ -1072,7 +1038,7 @@
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1"/>
       <c r="E14" s="7"/>
@@ -1083,26 +1049,18 @@
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1"/>
-      <c r="D15" s="9">
-        <v>4</v>
-      </c>
-      <c r="E15" s="7">
-        <v>1</v>
-      </c>
-      <c r="F15" s="9">
-        <v>2</v>
-      </c>
+      <c r="E15" s="7"/>
       <c r="O15" s="13">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="14"/>
@@ -1129,19 +1087,19 @@
       <c r="D17" s="11"/>
       <c r="E17" s="15">
         <f t="shared" ref="E17:N17" si="1">SUM(E3:E16)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F17" s="11">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="G17" s="11">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="11">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="11">
         <f t="shared" si="1"/>
@@ -1149,25 +1107,40 @@
       </c>
       <c r="J17" s="11">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" s="11">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L17" s="11">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="12"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>14</v>
       </c>
-      <c r="M17" s="11">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="N17" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="12"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1175,6 +1148,1131 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3B9CE9-F3CF-44FF-970A-67C2F787620D}">
+  <dimension ref="B2:R17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="9"/>
+    <col min="6" max="6" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="9.140625" style="9"/>
+    <col min="13" max="13" width="10.5703125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="9"/>
+    <col min="15" max="15" width="11.42578125" style="9" customWidth="1"/>
+    <col min="17" max="17" width="12" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="18">
+        <v>45962</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="9">
+        <v>42</v>
+      </c>
+      <c r="E3" s="7">
+        <v>3</v>
+      </c>
+      <c r="O3" s="13">
+        <f>SUM(F3:N3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="17">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="E4" s="7"/>
+      <c r="O4" s="13">
+        <f t="shared" ref="O4:O16" si="0">SUM(F4:N4)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="17">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="E5" s="7"/>
+      <c r="O5" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="9">
+        <v>40</v>
+      </c>
+      <c r="E6" s="7">
+        <v>2</v>
+      </c>
+      <c r="F6" s="9">
+        <v>6</v>
+      </c>
+      <c r="G6" s="9">
+        <v>2</v>
+      </c>
+      <c r="K6" s="9">
+        <v>2</v>
+      </c>
+      <c r="M6" s="9">
+        <v>1</v>
+      </c>
+      <c r="O6" s="13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="9">
+        <v>27</v>
+      </c>
+      <c r="E7" s="7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="9">
+        <v>4</v>
+      </c>
+      <c r="O7" s="13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="R7" s="9"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="E8" s="7"/>
+      <c r="O8" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="R8" s="10">
+        <f>SUM(F17:L17)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="E9" s="7"/>
+      <c r="O9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="R9" s="10">
+        <f>SUM(F17:G17)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="E10" s="7"/>
+      <c r="O10" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="R10" s="10">
+        <f>SUM(M17)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="E11" s="7"/>
+      <c r="O11" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="E12" s="7"/>
+      <c r="O12" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="E13" s="7"/>
+      <c r="O13" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="E14" s="7"/>
+      <c r="O14" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="E15" s="7"/>
+      <c r="O15" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="15">
+        <f t="shared" ref="E17:N17" si="1">SUM(E3:E16)</f>
+        <v>8</v>
+      </c>
+      <c r="F17" s="11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G17" s="11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="L17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE68A699-AE02-4412-ACDF-DCD7DCE0D211}">
+  <dimension ref="B2:R17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="9"/>
+    <col min="6" max="6" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="9.140625" style="9"/>
+    <col min="13" max="13" width="10.5703125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="9"/>
+    <col min="15" max="15" width="11.42578125" style="9" customWidth="1"/>
+    <col min="17" max="17" width="12" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="18">
+        <v>45959</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="9">
+        <v>42</v>
+      </c>
+      <c r="E3" s="7">
+        <v>3</v>
+      </c>
+      <c r="F3" s="9">
+        <v>5</v>
+      </c>
+      <c r="H3" s="9">
+        <v>1</v>
+      </c>
+      <c r="O3" s="13">
+        <f>SUM(F3:N3)</f>
+        <v>6</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="17"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="9">
+        <v>40</v>
+      </c>
+      <c r="E4" s="7">
+        <v>2</v>
+      </c>
+      <c r="F4" s="9">
+        <v>6</v>
+      </c>
+      <c r="O4" s="13">
+        <f t="shared" ref="O4:O16" si="0">SUM(F4:N4)</f>
+        <v>6</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="17"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="E5" s="7"/>
+      <c r="O5" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="E6" s="7"/>
+      <c r="O6" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="9">
+        <v>7</v>
+      </c>
+      <c r="E7" s="7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="9">
+        <v>2</v>
+      </c>
+      <c r="M7" s="9">
+        <v>1</v>
+      </c>
+      <c r="O7" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="R7" s="9"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="9">
+        <v>41</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="M8" s="9">
+        <v>1</v>
+      </c>
+      <c r="O8" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="R8" s="10">
+        <f>SUM(F17:L17)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="E9" s="7"/>
+      <c r="O9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="R9" s="10">
+        <f>SUM(F17:G17)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="E10" s="7"/>
+      <c r="O10" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="R10" s="10">
+        <f>SUM(M17)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="E11" s="7"/>
+      <c r="O11" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="9">
+        <v>18</v>
+      </c>
+      <c r="E12" s="7">
+        <v>2</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1</v>
+      </c>
+      <c r="O12" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="E13" s="7"/>
+      <c r="O13" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="E14" s="7"/>
+      <c r="O14" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="E15" s="7"/>
+      <c r="O15" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="15">
+        <f t="shared" ref="E17:N17" si="1">SUM(E3:E16)</f>
+        <v>10</v>
+      </c>
+      <c r="F17" s="11">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="G17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB60B8BE-3D50-4D47-9936-2650A3433373}">
+  <dimension ref="B2:R20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="9"/>
+    <col min="6" max="6" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="9.140625" style="9"/>
+    <col min="13" max="13" width="10.5703125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="9"/>
+    <col min="15" max="15" width="11.42578125" style="9" customWidth="1"/>
+    <col min="17" max="17" width="12" customWidth="1"/>
+    <col min="18" max="18" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="18">
+        <v>45956</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="9">
+        <v>18</v>
+      </c>
+      <c r="E3" s="7">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9">
+        <v>2</v>
+      </c>
+      <c r="I3" s="9">
+        <v>1</v>
+      </c>
+      <c r="K3" s="9">
+        <v>1</v>
+      </c>
+      <c r="O3" s="13">
+        <f>SUM(F3:N3)</f>
+        <v>4</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="17">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="E4" s="7"/>
+      <c r="O4" s="13">
+        <f t="shared" ref="O4:O16" si="0">SUM(F4:N4)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="17">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="E5" s="7"/>
+      <c r="O5" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="E6" s="7"/>
+      <c r="O6" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="E7" s="7"/>
+      <c r="O7" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="9"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="E8" s="7"/>
+      <c r="O8" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="R8" s="10">
+        <f>SUM(F17:L17)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="E9" s="7"/>
+      <c r="O9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="R9" s="10">
+        <f>SUM(F17:G17)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="E10" s="7"/>
+      <c r="O10" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="R10" s="10">
+        <f>SUM(M17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="E11" s="7"/>
+      <c r="O11" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="E12" s="7"/>
+      <c r="O12" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="E13" s="7"/>
+      <c r="O13" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="9">
+        <v>7</v>
+      </c>
+      <c r="E14" s="7">
+        <v>3</v>
+      </c>
+      <c r="F14" s="9">
+        <v>3</v>
+      </c>
+      <c r="G14" s="9">
+        <v>1</v>
+      </c>
+      <c r="L14" s="9">
+        <v>4</v>
+      </c>
+      <c r="O14" s="13">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="E15" s="7"/>
+      <c r="O15" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="15">
+        <f t="shared" ref="E17:N17" si="1">SUM(E3:E16)</f>
+        <v>5</v>
+      </c>
+      <c r="F17" s="11">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G17" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L17" s="11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="12"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6A20F9-24A1-4665-A386-F66C5BA9D520}">
   <dimension ref="B2:R17"/>
   <sheetViews>
@@ -1603,7 +2701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8BCD19A-3BA9-4EF2-BDF5-ACF1BF8CB3B3}">
   <dimension ref="B2:R17"/>
   <sheetViews>
@@ -2004,7 +3102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1A4CEB5-BF15-4E07-A8BC-7567CA4D9501}">
   <dimension ref="B2:R17"/>
   <sheetViews>
@@ -2475,7 +3573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B332F4-D8C2-411F-AA39-D3B192007917}">
   <dimension ref="B2:R17"/>
   <sheetViews>
@@ -2983,7 +4081,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4C505A-A53F-423E-8CC6-A18CF8A5CBA2}">
   <dimension ref="B2:R17"/>
   <sheetViews>
@@ -3311,6 +4409,1181 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC73AB3-3A95-45D5-8542-1E3ACB06E9FC}">
+  <dimension ref="B2:R17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="9"/>
+    <col min="6" max="6" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="9.140625" style="9"/>
+    <col min="13" max="13" width="10.5703125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="9"/>
+    <col min="15" max="15" width="11.42578125" style="9" customWidth="1"/>
+    <col min="17" max="17" width="12" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="18">
+        <v>45980</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="9">
+        <v>25</v>
+      </c>
+      <c r="E3" s="7">
+        <v>2</v>
+      </c>
+      <c r="L3" s="9">
+        <v>2</v>
+      </c>
+      <c r="O3" s="13">
+        <f>SUM(F3:N3)</f>
+        <v>2</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="17">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="E4" s="7"/>
+      <c r="O4" s="13">
+        <f t="shared" ref="O4:O16" si="0">SUM(F4:N4)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="17">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="E5" s="7"/>
+      <c r="O5" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="E6" s="7"/>
+      <c r="O6" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="9">
+        <v>40</v>
+      </c>
+      <c r="E7" s="7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="9">
+        <v>2</v>
+      </c>
+      <c r="K7" s="9">
+        <v>2</v>
+      </c>
+      <c r="O7" s="13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="R7" s="9"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="E8" s="7"/>
+      <c r="O8" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="R8" s="10">
+        <f>SUM(F17:L17)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="E9" s="7"/>
+      <c r="O9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="R9" s="10">
+        <f>SUM(F17:G17)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="E10" s="7"/>
+      <c r="O10" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="R10" s="10">
+        <f>SUM(M17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="E11" s="7"/>
+      <c r="O11" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="E12" s="7"/>
+      <c r="O12" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="9">
+        <v>7</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1</v>
+      </c>
+      <c r="F13" s="9">
+        <v>3</v>
+      </c>
+      <c r="G13" s="9">
+        <v>1</v>
+      </c>
+      <c r="L13" s="9">
+        <v>1</v>
+      </c>
+      <c r="O13" s="13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="E14" s="7"/>
+      <c r="O14" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="E15" s="7"/>
+      <c r="O15" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="14">
+        <v>42</v>
+      </c>
+      <c r="E16" s="8">
+        <v>2</v>
+      </c>
+      <c r="F16" s="14">
+        <v>6</v>
+      </c>
+      <c r="G16" s="14">
+        <v>2</v>
+      </c>
+      <c r="H16" s="14">
+        <v>1</v>
+      </c>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14">
+        <v>1</v>
+      </c>
+      <c r="L16" s="14">
+        <v>3</v>
+      </c>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="13">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="15">
+        <f t="shared" ref="E17:N17" si="1">SUM(E3:E16)</f>
+        <v>7</v>
+      </c>
+      <c r="F17" s="11">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G17" s="11">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="11">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="L17" s="11">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="M17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01AC2C32-5460-4EF5-9733-4D3358B4AFEE}">
+  <dimension ref="B2:R21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="9"/>
+    <col min="6" max="6" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="9.140625" style="9"/>
+    <col min="13" max="13" width="10.5703125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="9"/>
+    <col min="15" max="15" width="11.42578125" style="9" customWidth="1"/>
+    <col min="17" max="17" width="12" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="18">
+        <v>45977</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="9">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7">
+        <v>3</v>
+      </c>
+      <c r="F3" s="9">
+        <v>3</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9">
+        <v>8</v>
+      </c>
+      <c r="L3" s="9">
+        <v>9</v>
+      </c>
+      <c r="O3" s="13">
+        <f>SUM(F3:N3)</f>
+        <v>21</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="17">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="9">
+        <v>40</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="9">
+        <v>6</v>
+      </c>
+      <c r="K4" s="9">
+        <v>1</v>
+      </c>
+      <c r="O4" s="13">
+        <f t="shared" ref="O4:O16" si="0">SUM(F4:N4)</f>
+        <v>7</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="17">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="E5" s="7"/>
+      <c r="O5" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="E6" s="7"/>
+      <c r="O6" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="E7" s="7"/>
+      <c r="O7" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="9"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="9">
+        <v>27</v>
+      </c>
+      <c r="E8" s="7">
+        <v>2</v>
+      </c>
+      <c r="G8" s="9">
+        <v>2</v>
+      </c>
+      <c r="O8" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="R8" s="10">
+        <f>SUM(F17:L17)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="E9" s="7"/>
+      <c r="O9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="R9" s="10">
+        <f>SUM(F17:G17)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="E10" s="7"/>
+      <c r="O10" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="R10" s="10">
+        <f>SUM(M17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="E11" s="7"/>
+      <c r="O11" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="E12" s="7"/>
+      <c r="O12" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="E13" s="7"/>
+      <c r="O13" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="E14" s="7"/>
+      <c r="O14" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="E15" s="7"/>
+      <c r="O15" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="15">
+        <f t="shared" ref="E17:N17" si="1">SUM(E3:E16)</f>
+        <v>6</v>
+      </c>
+      <c r="F17" s="11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G17" s="11">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="11">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L17" s="11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="M17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="12"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCD1FAE-E10A-49B0-9459-DEB3D3947B05}">
+  <dimension ref="B2:R17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="9"/>
+    <col min="6" max="6" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="9.140625" style="9"/>
+    <col min="13" max="13" width="10.5703125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="9"/>
+    <col min="15" max="15" width="11.42578125" style="9" customWidth="1"/>
+    <col min="17" max="17" width="12" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="18">
+        <v>45976</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="E3" s="7"/>
+      <c r="O3" s="13">
+        <f>SUM(F3:N3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="17">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="E4" s="7"/>
+      <c r="O4" s="13">
+        <f t="shared" ref="O4:O16" si="0">SUM(F4:N4)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="17">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="9">
+        <v>7</v>
+      </c>
+      <c r="E5" s="7">
+        <v>2</v>
+      </c>
+      <c r="F5" s="9">
+        <v>14</v>
+      </c>
+      <c r="O5" s="13">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="9">
+        <v>41</v>
+      </c>
+      <c r="E6" s="7">
+        <v>4</v>
+      </c>
+      <c r="F6" s="9">
+        <v>3</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="9">
+        <v>1</v>
+      </c>
+      <c r="L6" s="9">
+        <v>3</v>
+      </c>
+      <c r="M6" s="9">
+        <v>2</v>
+      </c>
+      <c r="O6" s="13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="9">
+        <v>18</v>
+      </c>
+      <c r="E7" s="7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="9">
+        <v>2</v>
+      </c>
+      <c r="J7" s="9">
+        <v>1</v>
+      </c>
+      <c r="K7" s="9">
+        <v>2</v>
+      </c>
+      <c r="L7" s="9">
+        <v>9</v>
+      </c>
+      <c r="O7" s="13">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="R7" s="9"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="9">
+        <v>42</v>
+      </c>
+      <c r="E8" s="7">
+        <v>2</v>
+      </c>
+      <c r="F8" s="9">
+        <v>5</v>
+      </c>
+      <c r="L8" s="9">
+        <v>2</v>
+      </c>
+      <c r="O8" s="13">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="R8" s="10">
+        <f>SUM(F17:L17)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="E9" s="7"/>
+      <c r="O9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="R9" s="10">
+        <f>SUM(F17:G17)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="E10" s="7"/>
+      <c r="O10" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="R10" s="10">
+        <f>SUM(M17)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="E11" s="7"/>
+      <c r="O11" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="E12" s="7"/>
+      <c r="O12" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="E13" s="7"/>
+      <c r="O13" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="E14" s="7"/>
+      <c r="O14" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="9">
+        <v>4</v>
+      </c>
+      <c r="E15" s="7">
+        <v>1</v>
+      </c>
+      <c r="F15" s="9">
+        <v>2</v>
+      </c>
+      <c r="O15" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="15">
+        <f t="shared" ref="E17:N17" si="1">SUM(E3:E16)</f>
+        <v>12</v>
+      </c>
+      <c r="F17" s="11">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="G17" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K17" s="11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="L17" s="11">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="M17" s="11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD94C4D-3A8E-42E8-B85D-CEE219656498}">
   <dimension ref="B2:R17"/>
   <sheetViews>
@@ -3671,7 +5944,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD6B12EE-1808-4D81-9182-A53CAFA0C601}">
   <dimension ref="B2:R18"/>
   <sheetViews>
@@ -4039,7 +6312,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9002B072-BCCF-45C1-B367-C74FA3B590EA}">
   <dimension ref="B2:R18"/>
   <sheetViews>
@@ -4414,7 +6687,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF33574-73DD-4615-A28D-599866F62919}">
   <dimension ref="B2:R17"/>
   <sheetViews>
@@ -4820,7 +7093,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDC3552-07C9-4ED5-B498-126CAAA60F55}">
   <dimension ref="B2:R17"/>
   <sheetViews>
@@ -5166,1129 +7439,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3B9CE9-F3CF-44FF-970A-67C2F787620D}">
-  <dimension ref="B2:R17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="9"/>
-    <col min="6" max="6" width="12" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="9.140625" style="9"/>
-    <col min="13" max="13" width="10.5703125" style="9" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="9"/>
-    <col min="15" max="15" width="11.42578125" style="9" customWidth="1"/>
-    <col min="17" max="17" width="12" customWidth="1"/>
-    <col min="18" max="18" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2" s="18">
-        <v>45962</v>
-      </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="9">
-        <v>42</v>
-      </c>
-      <c r="E3" s="7">
-        <v>3</v>
-      </c>
-      <c r="O3" s="13">
-        <f>SUM(F3:N3)</f>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R3" s="17">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="E4" s="7"/>
-      <c r="O4" s="13">
-        <f t="shared" ref="O4:O16" si="0">SUM(F4:N4)</f>
-        <v>0</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" s="17">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="E5" s="7"/>
-      <c r="O5" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="R5" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="9">
-        <v>40</v>
-      </c>
-      <c r="E6" s="7">
-        <v>2</v>
-      </c>
-      <c r="F6" s="9">
-        <v>6</v>
-      </c>
-      <c r="G6" s="9">
-        <v>2</v>
-      </c>
-      <c r="K6" s="9">
-        <v>2</v>
-      </c>
-      <c r="M6" s="9">
-        <v>1</v>
-      </c>
-      <c r="O6" s="13">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="R6" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="9">
-        <v>27</v>
-      </c>
-      <c r="E7" s="7">
-        <v>3</v>
-      </c>
-      <c r="F7" s="9">
-        <v>4</v>
-      </c>
-      <c r="O7" s="13">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="R7" s="9"/>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="E8" s="7"/>
-      <c r="O8" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="R8" s="10">
-        <f>SUM(F17:L17)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="E9" s="7"/>
-      <c r="O9" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="R9" s="10">
-        <f>SUM(F17:G17)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="E10" s="7"/>
-      <c r="O10" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="R10" s="10">
-        <f>SUM(M17)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="E11" s="7"/>
-      <c r="O11" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="E12" s="7"/>
-      <c r="O12" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="E13" s="7"/>
-      <c r="O13" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="E14" s="7"/>
-      <c r="O14" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="E15" s="7"/>
-      <c r="O15" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="15">
-        <f t="shared" ref="E17:N17" si="1">SUM(E3:E16)</f>
-        <v>8</v>
-      </c>
-      <c r="F17" s="11">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="G17" s="11">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H17" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="11">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="L17" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M17" s="11">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="N17" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE68A699-AE02-4412-ACDF-DCD7DCE0D211}">
-  <dimension ref="B2:R17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="9"/>
-    <col min="6" max="6" width="12" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="9.140625" style="9"/>
-    <col min="13" max="13" width="10.5703125" style="9" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="9"/>
-    <col min="15" max="15" width="11.42578125" style="9" customWidth="1"/>
-    <col min="17" max="17" width="12" customWidth="1"/>
-    <col min="18" max="18" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2" s="18">
-        <v>45959</v>
-      </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="9">
-        <v>42</v>
-      </c>
-      <c r="E3" s="7">
-        <v>3</v>
-      </c>
-      <c r="F3" s="9">
-        <v>5</v>
-      </c>
-      <c r="H3" s="9">
-        <v>1</v>
-      </c>
-      <c r="O3" s="13">
-        <f>SUM(F3:N3)</f>
-        <v>6</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R3" s="17"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="9">
-        <v>40</v>
-      </c>
-      <c r="E4" s="7">
-        <v>2</v>
-      </c>
-      <c r="F4" s="9">
-        <v>6</v>
-      </c>
-      <c r="O4" s="13">
-        <f t="shared" ref="O4:O16" si="0">SUM(F4:N4)</f>
-        <v>6</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" s="17"/>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="E5" s="7"/>
-      <c r="O5" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="R5" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="E6" s="7"/>
-      <c r="O6" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="R6" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="9">
-        <v>7</v>
-      </c>
-      <c r="E7" s="7">
-        <v>2</v>
-      </c>
-      <c r="F7" s="9">
-        <v>2</v>
-      </c>
-      <c r="M7" s="9">
-        <v>1</v>
-      </c>
-      <c r="O7" s="13">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R7" s="9"/>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="9">
-        <v>41</v>
-      </c>
-      <c r="E8" s="7">
-        <v>1</v>
-      </c>
-      <c r="M8" s="9">
-        <v>1</v>
-      </c>
-      <c r="O8" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Q8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="R8" s="10">
-        <f>SUM(F17:L17)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="E9" s="7"/>
-      <c r="O9" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="R9" s="10">
-        <f>SUM(F17:G17)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="E10" s="7"/>
-      <c r="O10" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="R10" s="10">
-        <f>SUM(M17)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="E11" s="7"/>
-      <c r="O11" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="9">
-        <v>18</v>
-      </c>
-      <c r="E12" s="7">
-        <v>2</v>
-      </c>
-      <c r="F12" s="9">
-        <v>1</v>
-      </c>
-      <c r="O12" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="E13" s="7"/>
-      <c r="O13" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="E14" s="7"/>
-      <c r="O14" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="E15" s="7"/>
-      <c r="O15" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="15">
-        <f t="shared" ref="E17:N17" si="1">SUM(E3:E16)</f>
-        <v>10</v>
-      </c>
-      <c r="F17" s="11">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="G17" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="11">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I17" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L17" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M17" s="11">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="N17" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB60B8BE-3D50-4D47-9936-2650A3433373}">
-  <dimension ref="B2:R20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="9"/>
-    <col min="6" max="6" width="12" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="9.140625" style="9"/>
-    <col min="13" max="13" width="10.5703125" style="9" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="9"/>
-    <col min="15" max="15" width="11.42578125" style="9" customWidth="1"/>
-    <col min="17" max="17" width="12" customWidth="1"/>
-    <col min="18" max="18" width="19.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2" s="18">
-        <v>45956</v>
-      </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="9">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7">
-        <v>2</v>
-      </c>
-      <c r="F3" s="9">
-        <v>2</v>
-      </c>
-      <c r="I3" s="9">
-        <v>1</v>
-      </c>
-      <c r="K3" s="9">
-        <v>1</v>
-      </c>
-      <c r="O3" s="13">
-        <f>SUM(F3:N3)</f>
-        <v>4</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R3" s="17">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="E4" s="7"/>
-      <c r="O4" s="13">
-        <f t="shared" ref="O4:O16" si="0">SUM(F4:N4)</f>
-        <v>0</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" s="17">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="E5" s="7"/>
-      <c r="O5" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="R5" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="E6" s="7"/>
-      <c r="O6" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="R6" s="17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="E7" s="7"/>
-      <c r="O7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="9"/>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="E8" s="7"/>
-      <c r="O8" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="R8" s="10">
-        <f>SUM(F17:L17)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="E9" s="7"/>
-      <c r="O9" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="R9" s="10">
-        <f>SUM(F17:G17)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="E10" s="7"/>
-      <c r="O10" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="R10" s="10">
-        <f>SUM(M17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="E11" s="7"/>
-      <c r="O11" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="E12" s="7"/>
-      <c r="O12" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="E13" s="7"/>
-      <c r="O13" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="9">
-        <v>7</v>
-      </c>
-      <c r="E14" s="7">
-        <v>3</v>
-      </c>
-      <c r="F14" s="9">
-        <v>3</v>
-      </c>
-      <c r="G14" s="9">
-        <v>1</v>
-      </c>
-      <c r="L14" s="9">
-        <v>4</v>
-      </c>
-      <c r="O14" s="13">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="E15" s="7"/>
-      <c r="O15" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="15">
-        <f t="shared" ref="E17:N17" si="1">SUM(E3:E16)</f>
-        <v>5</v>
-      </c>
-      <c r="F17" s="11">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="G17" s="11">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H17" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="11">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J17" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="11">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L17" s="11">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="M17" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N17" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="12"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update analytics dashboard and individual member stats with improved UI, charts, and data visualization
</commit_message>
<xml_diff>
--- a/LOGC_Tracker.xlsx
+++ b/LOGC_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a9153f6611ebe33/Documents/Hunting Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="583" documentId="8_{29F3ABBB-D82D-4D93-83B8-9233ECB04D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C27C0E88-2314-4329-B9C2-696C8028480F}"/>
+  <xr:revisionPtr revIDLastSave="585" documentId="8_{29F3ABBB-D82D-4D93-83B8-9233ECB04D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC412AB5-7780-43DC-B649-5FC7D300096F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{FDA17AAC-9089-415D-B005-ED1660AC87E8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="13" xr2:uid="{FDA17AAC-9089-415D-B005-ED1660AC87E8}"/>
   </bookViews>
   <sheets>
     <sheet name="11_22_25 TODO" sheetId="18" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="61">
   <si>
     <t>Member</t>
   </si>
@@ -193,9 +193,6 @@
   </si>
   <si>
     <t>SSE 4-7 mph</t>
-  </si>
-  <si>
-    <t>Gray Dome</t>
   </si>
   <si>
     <t>SSE 14 mph</t>
@@ -789,7 +786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7548CB-591B-437C-829E-1AFE6F4F8FA2}">
   <dimension ref="B2:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
@@ -1274,7 +1271,7 @@
         <v>30</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -1653,7 +1650,7 @@
         <v>30</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -1670,7 +1667,7 @@
         <v>31</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
@@ -2031,7 +2028,7 @@
         <v>30</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -2048,7 +2045,7 @@
         <v>31</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
@@ -2705,8 +2702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8BCD19A-3BA9-4EF2-BDF5-ACF1BF8CB3B3}">
   <dimension ref="B2:R17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2851,7 +2848,7 @@
         <v>31</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
@@ -4413,7 +4410,7 @@
   <dimension ref="B2:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4555,7 +4552,7 @@
         <v>31</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
@@ -4794,10 +4791,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01AC2C32-5460-4EF5-9733-4D3358B4AFEE}">
-  <dimension ref="B2:R21"/>
+  <dimension ref="B2:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4944,7 +4941,7 @@
         <v>30</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -4961,7 +4958,7 @@
         <v>31</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
@@ -5161,21 +5158,6 @@
         <v>0</v>
       </c>
       <c r="O17" s="12"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>26</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5312,7 +5294,7 @@
         <v>30</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -5718,7 +5700,7 @@
         <v>30</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -5735,7 +5717,7 @@
         <v>31</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
@@ -6228,7 +6210,7 @@
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="14">
@@ -6842,7 +6824,7 @@
         <v>30</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -6859,7 +6841,7 @@
         <v>31</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">

</xml_diff>